<commit_message>
Edits made to excel and mathematica file
</commit_message>
<xml_diff>
--- a/PopulationModeling/PopulationProjectGraphs.xlsx
+++ b/PopulationModeling/PopulationProjectGraphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Towson\SeniorYear\FallSemester\MATH377\MathematicalModels\PopulationModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25C4837-8E85-44DA-8E1F-0D93BC3D75D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D9EF99-65A8-45D4-8989-AA997DDFCD3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{4613FAD3-24D1-4C69-977E-63F0B20BB996}"/>
   </bookViews>
@@ -217,6 +217,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Luvmee Population</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1869,6 +1894,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Luvmee Population</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4999,8 +5049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5B6FA1-1032-4F8D-89B9-CE6A41533FF7}">
   <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J12" workbookViewId="0">
-      <selection sqref="A1:AF7"/>
+    <sheetView tabSelected="1" topLeftCell="S7" workbookViewId="0">
+      <selection activeCell="AI8" sqref="AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>